<commit_message>
Markov initial file - axis error not fixed yet + sport tracker updated
</commit_message>
<xml_diff>
--- a/Sport Tracker/Natation.xlsx
+++ b/Sport Tracker/Natation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\OneDrive\The Eggcellent\Coding Projects\2024\Manim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\OneDrive\The Eggcellent\Coding Projects\2024\Manim\Sport Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE42D6B1-D119-4191-B048-BC3C7D276517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD41318A-9408-4F82-9796-57154DCD6841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,13 +30,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Grossed distance</t>
-  </si>
-  <si>
     <t>KPI</t>
   </si>
   <si>
     <t>Session</t>
+  </si>
+  <si>
+    <t>Grossed distance (m)</t>
   </si>
 </sst>
 </file>
@@ -177,7 +177,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Grossed distance</c:v>
+                  <c:v>Grossed distance (m)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -209,6 +209,9 @@
                   <c:pt idx="0">
                     <c:v>27/08/2024</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30/08/2024</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -271,6 +274,9 @@
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -323,6 +329,9 @@
                   <c:pt idx="0">
                     <c:v>27/08/2024</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30/08/2024</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -387,49 +396,49 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1100</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1200</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1300</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1400</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1500</c:v>
+                  <c:v>2300</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1600</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1700</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1800</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1900</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2100</c:v>
+                  <c:v>2900</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2200</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2300</c:v>
+                  <c:v>3100</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2400</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2500</c:v>
+                  <c:v>3300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1485,7 +1494,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1497,16 +1506,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1527,8 +1536,14 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" s="1">
+        <v>45534</v>
+      </c>
+      <c r="C3">
+        <v>2000</v>
+      </c>
       <c r="D3">
-        <v>1100</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1536,7 +1551,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>1200</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1544,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>1300</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1552,7 +1567,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>1400</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1560,7 +1575,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>1500</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1568,7 +1583,7 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>1600</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1576,7 +1591,7 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>1700</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1584,7 +1599,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>1800</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1592,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>1900</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1600,7 +1615,7 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>2000</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1608,7 +1623,7 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>2100</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1616,7 +1631,7 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>2200</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1624,7 +1639,7 @@
         <v>14</v>
       </c>
       <c r="D15">
-        <v>2300</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1632,7 +1647,7 @@
         <v>15</v>
       </c>
       <c r="D16">
-        <v>2400</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1640,7 +1655,7 @@
         <v>16</v>
       </c>
       <c r="D17">
-        <v>2500</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>